<commit_message>
Typo in Group 4 scores corrected
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/Face2Face/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD3574E-6444-DA49-B649-3FBFFF321EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8269AB5C-68C4-9647-9EED-BF34B373B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967CD6C7-451E-0748-9748-9A42CF32D73A}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,7 +764,7 @@
       </c>
       <c r="P2" s="20">
         <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>-29.832212517316719</v>
+        <v>0.19900638614136706</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -1031,7 +1031,7 @@
         <v>10.10225</v>
       </c>
       <c r="I13" s="16">
-        <v>1.9179999999999999E-2</v>
+        <v>0.1017933</v>
       </c>
       <c r="J13" s="24">
         <v>10.233549999999999</v>
@@ -1459,7 +1459,7 @@
       <c r="G25" s="18"/>
       <c r="H25" s="20">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), H13, I13, 0 ) )</f>
-        <v>-29.832212517316719</v>
+        <v>0.19900638614136706</v>
       </c>
       <c r="I25" s="20"/>
       <c r="J25" s="18">

</xml_diff>

<commit_message>
Second Round Scores & third round forecasts
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/Face2Face/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8269AB5C-68C4-9647-9EED-BF34B373B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACDFEC7-D813-3546-BDEC-1CCBBC7AA288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="36600" yWindow="-2400" windowWidth="30420" windowHeight="17080" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -243,7 +243,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -307,8 +307,8 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,46 +648,46 @@
         <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="20"/>
       <c r="R1" s="20"/>
@@ -706,65 +706,65 @@
       <c r="A2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="16">
         <f>SUMIF($T25:$T34,"&lt;&gt;#NUM!")</f>
-        <v>2.411491593688377</v>
-      </c>
-      <c r="C2" s="20">
+        <v>5.0906686392411391</v>
+      </c>
+      <c r="C2" s="16">
+        <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
+        <v>4.3527625719855481</v>
+      </c>
+      <c r="D2" s="16">
+        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
+        <v>3.9286173327671841</v>
+      </c>
+      <c r="E2" s="16">
         <f>SUMIF($N25:$N34,"&lt;&gt;#NUM!")</f>
-        <v>1.9855577193589098</v>
-      </c>
-      <c r="D2" s="20">
-        <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
-        <v>1.9691952826678027</v>
-      </c>
-      <c r="E2" s="20">
-        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
-        <v>1.967043831873476</v>
-      </c>
-      <c r="F2" s="20">
+        <v>3.7064852830732433</v>
+      </c>
+      <c r="F2" s="16">
+        <f>SUMIF($AD25:$AD34,"&lt;&gt;#NUM!")</f>
+        <v>3.5491634006341246</v>
+      </c>
+      <c r="G2" s="16">
         <f>SUMIF($J25:$J34,"&lt;&gt;#NUM!")</f>
-        <v>1.8219182385525092</v>
-      </c>
-      <c r="G2" s="20">
+        <v>3.3075953960677391</v>
+      </c>
+      <c r="H2" s="16">
         <f>SUMIF($Z25:$Z34,"&lt;&gt;#NUM!")</f>
-        <v>1.5429788757167571</v>
-      </c>
-      <c r="H2" s="20">
-        <f>SUMIF($AD25:$AD34,"&lt;&gt;#NUM!")</f>
-        <v>1.4680077209757174</v>
-      </c>
-      <c r="I2" s="20">
+        <v>2.8763930119347028</v>
+      </c>
+      <c r="I2" s="16">
+        <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
+        <v>2.860575398203661</v>
+      </c>
+      <c r="J2" s="16">
         <f>SUMIF($D25:$D34,"&lt;&gt;#NUM!")</f>
-        <v>1.3817063066455832</v>
-      </c>
-      <c r="J2" s="20">
-        <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
-        <v>1.3711438977342807</v>
-      </c>
-      <c r="K2" s="20">
+        <v>2.8045286082909602</v>
+      </c>
+      <c r="K2" s="16">
         <f>SUMIF($L25:$L34,"&lt;&gt;#NUM!")</f>
-        <v>1.3393279650215224</v>
-      </c>
-      <c r="L2" s="20">
+        <v>2.6489868428226888</v>
+      </c>
+      <c r="L2" s="16">
+        <f>SUMIF($X25:$X34,"&lt;&gt;#NUM!")</f>
+        <v>2.2360650816493983</v>
+      </c>
+      <c r="M2" s="16">
+        <f>SUMIF($R25:$R34,"&lt;&gt;#NUM!")</f>
+        <v>2.1851352372883657</v>
+      </c>
+      <c r="N2" s="16">
+        <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
+        <v>1.9982847302212812</v>
+      </c>
+      <c r="O2" s="16">
+        <f>SUMIF($AB25:$AB34,"&lt;&gt;#NUM!")</f>
+        <v>1.7467996514738675</v>
+      </c>
+      <c r="P2" s="16">
         <f>SUMIF($V25:$V34,"&lt;&gt;#NUM!")</f>
-        <v>1.2965615460910569</v>
-      </c>
-      <c r="M2" s="20">
-        <f>SUMIF($R25:$R34,"&lt;&gt;#NUM!")</f>
-        <v>0.94873942156195867</v>
-      </c>
-      <c r="N2" s="20">
-        <f>SUMIF($X25:$X34,"&lt;&gt;#NUM!")</f>
-        <v>0.91567814574715556</v>
-      </c>
-      <c r="O2" s="20">
-        <f>SUMIF($AB25:$AB34,"&lt;&gt;#NUM!")</f>
-        <v>0.73976437341199108</v>
-      </c>
-      <c r="P2" s="20">
-        <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>0.19900638614136706</v>
+        <v>1.2914767145907713</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -1033,10 +1033,10 @@
       <c r="I13" s="16">
         <v>0.1017933</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="11">
         <v>10.233549999999999</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="11">
         <v>5.9369999999999999E-2</v>
       </c>
       <c r="L13" s="4">
@@ -1051,7 +1051,7 @@
       <c r="O13" s="10">
         <v>5.2329924722341999E-2</v>
       </c>
-      <c r="P13" s="26">
+      <c r="P13" s="28">
         <v>10.28497</v>
       </c>
       <c r="Q13" s="4">
@@ -1063,7 +1063,7 @@
       <c r="S13" s="10">
         <v>4.6036359999999998E-2</v>
       </c>
-      <c r="T13" s="26">
+      <c r="T13" s="28">
         <v>10.259888249999999</v>
       </c>
       <c r="U13" s="4">
@@ -1075,7 +1075,7 @@
       <c r="W13" s="10">
         <v>9.6529813811318199E-2</v>
       </c>
-      <c r="X13" s="26">
+      <c r="X13" s="28">
         <v>10.291</v>
       </c>
       <c r="Y13" s="4">
@@ -1087,7 +1087,7 @@
       <c r="AA13" s="10">
         <v>6.6113560000000002E-2</v>
       </c>
-      <c r="AB13" s="26">
+      <c r="AB13" s="28">
         <v>10.143990000000001</v>
       </c>
       <c r="AC13" s="4">
@@ -1099,10 +1099,10 @@
       <c r="AE13" s="10">
         <v>7.4385259999999995E-2</v>
       </c>
-      <c r="AJ13" s="28" t="s">
+      <c r="AJ13" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AK13">
+      <c r="AK13" s="3">
         <v>28502.729166666672</v>
       </c>
     </row>
@@ -1110,63 +1110,198 @@
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AJ14" s="28" t="s">
+      <c r="B14" s="10">
+        <v>10.22438</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3.5883289999999998E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10.205</v>
+      </c>
+      <c r="E14" s="4">
+        <v>9.5479999999999995E-2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>10.2411010108677</v>
+      </c>
+      <c r="G14" s="10">
+        <v>4.9523730728451398E-2</v>
+      </c>
+      <c r="H14" s="15">
+        <v>10.21006</v>
+      </c>
+      <c r="I14" s="15">
+        <v>6.5689540000000005E-2</v>
+      </c>
+      <c r="J14" s="11">
+        <v>10.27074</v>
+      </c>
+      <c r="K14" s="11">
+        <v>5.9319999999999998E-2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>10.165749999999999</v>
+      </c>
+      <c r="M14" s="3">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="N14" s="10">
+        <v>10.2576110782105</v>
+      </c>
+      <c r="O14" s="10">
+        <v>5.22771757102648E-2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>10.233560000000001</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>8.8270000000000001E-2</v>
+      </c>
+      <c r="R14" s="10">
+        <v>10.27891</v>
+      </c>
+      <c r="S14" s="10">
+        <v>4.603964E-2</v>
+      </c>
+      <c r="T14" s="4">
+        <v>10.22036589</v>
+      </c>
+      <c r="U14" s="4">
+        <v>2.70772858823576E-2</v>
+      </c>
+      <c r="V14" s="10">
+        <v>10.328430000000001</v>
+      </c>
+      <c r="W14" s="10">
+        <v>5.6646259999999997E-2</v>
+      </c>
+      <c r="X14" s="4">
+        <v>10.269242999999999</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>3.5816790000000001E-2</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>10.280049999999999</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>6.6124440000000007E-2</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>10.1296</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>0.10009999999999999</v>
+      </c>
+      <c r="AD14" s="10">
+        <v>10.23602</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>4.5309839999999997E-2</v>
+      </c>
+      <c r="AJ14" s="27" t="s">
         <v>30</v>
+      </c>
+      <c r="AK14" s="3">
+        <v>27346.9375</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AJ15" s="28" t="s">
+      <c r="B15" s="11">
+        <v>10.08137</v>
+      </c>
+      <c r="C15" s="11">
+        <v>3.5753470000000002E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>10.146000000000001</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3.0849999999999999E-2</v>
+      </c>
+      <c r="F15" s="11">
+        <v>10.13245989821</v>
+      </c>
+      <c r="G15" s="11">
+        <v>4.30765154025032E-2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>10.10017</v>
+      </c>
+      <c r="I15" s="16">
+        <v>4.4511149999999999E-2</v>
+      </c>
+      <c r="J15" s="11">
+        <v>10.103669999999999</v>
+      </c>
+      <c r="K15" s="11">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="L15" s="3">
+        <v>10.093819999999999</v>
+      </c>
+      <c r="M15" s="3">
+        <v>6.2799999999999995E-2</v>
+      </c>
+      <c r="N15" s="11">
+        <v>10.2396810130661</v>
+      </c>
+      <c r="O15" s="11">
+        <v>5.2258460684578699E-2</v>
+      </c>
+      <c r="P15" s="3">
+        <v>10.157590000000001</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>6.6600000000000006E-2</v>
+      </c>
+      <c r="R15" s="11">
+        <v>10.179779999999999</v>
+      </c>
+      <c r="S15" s="11">
+        <v>4.6028060000000003E-2</v>
+      </c>
+      <c r="T15" s="16">
+        <v>10.18139388</v>
+      </c>
+      <c r="U15" s="16">
+        <v>4.7947320425839497E-2</v>
+      </c>
+      <c r="V15" s="11">
+        <v>10.2136</v>
+      </c>
+      <c r="W15" s="11">
+        <v>4.1760039999999998E-2</v>
+      </c>
+      <c r="X15" s="16">
+        <v>10.167612</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>1.48261709E-2</v>
+      </c>
+      <c r="Z15" s="11">
+        <v>10.16825</v>
+      </c>
+      <c r="AA15" s="11">
+        <v>5.6398139999999999E-2</v>
+      </c>
+      <c r="AB15" s="16">
+        <v>10.14</v>
+      </c>
+      <c r="AC15" s="16">
+        <v>9.9199999999999997E-2</v>
+      </c>
+      <c r="AD15" s="11">
+        <v>10.14744</v>
+      </c>
+      <c r="AE15" s="11">
+        <v>4.5327600000000003E-2</v>
+      </c>
+      <c r="AJ15" s="27" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1182,7 +1317,7 @@
       <c r="I16" s="20"/>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
-      <c r="M16" s="27"/>
+      <c r="M16" s="26"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
       <c r="R16" s="18"/>
@@ -1193,7 +1328,7 @@
       <c r="AA16" s="18"/>
       <c r="AD16" s="18"/>
       <c r="AE16" s="18"/>
-      <c r="AJ16" s="28" t="s">
+      <c r="AJ16" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1219,7 +1354,7 @@
       <c r="AA17" s="18"/>
       <c r="AD17" s="18"/>
       <c r="AE17" s="18"/>
-      <c r="AJ17" s="28" t="s">
+      <c r="AJ17" s="27" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1255,7 +1390,7 @@
       <c r="AC18" s="20"/>
       <c r="AD18" s="18"/>
       <c r="AE18" s="18"/>
-      <c r="AJ18" s="28" t="s">
+      <c r="AJ18" s="27" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1279,7 +1414,7 @@
       <c r="AA19" s="18"/>
       <c r="AD19" s="18"/>
       <c r="AE19" s="18"/>
-      <c r="AJ19" s="28" t="s">
+      <c r="AJ19" s="27" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1307,7 +1442,7 @@
       <c r="AA20" s="18"/>
       <c r="AD20" s="18"/>
       <c r="AE20" s="18"/>
-      <c r="AJ20" s="28" t="s">
+      <c r="AJ20" s="27" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1442,154 +1577,161 @@
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), B13, C13, 0 ) )</f>
         <v>1.9691952826678027</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="20">
+      <c r="C25" s="11"/>
+      <c r="D25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), D13, E13, 0 ) )</f>
         <v>1.3817063066455832</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="18">
+      <c r="E25" s="16"/>
+      <c r="F25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), F13, G13, 0 ) )</f>
         <v>1.967043831873476</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="20">
+      <c r="G25" s="11"/>
+      <c r="H25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), H13, I13, 0 ) )</f>
         <v>0.19900638614136706</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="18">
+      <c r="I25" s="16"/>
+      <c r="J25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), J13, K13, 0 ) )</f>
         <v>1.8219182385525092</v>
       </c>
-      <c r="K25" s="18"/>
-      <c r="L25" s="20">
+      <c r="K25" s="11"/>
+      <c r="L25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), L13, M13, 0 ) )</f>
         <v>1.3393279650215224</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="18">
+      <c r="M25" s="16"/>
+      <c r="N25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), N13, O13, 0 ) )</f>
         <v>1.9855577193589098</v>
       </c>
-      <c r="O25" s="18"/>
-      <c r="P25" s="20">
+      <c r="O25" s="11"/>
+      <c r="P25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), P13, Q13, 0 ) )</f>
         <v>1.3711438977342807</v>
       </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="18">
+      <c r="Q25" s="16"/>
+      <c r="R25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), R13, S13, 0 ) )</f>
         <v>0.94873942156195867</v>
       </c>
-      <c r="S25" s="18"/>
-      <c r="T25" s="20">
+      <c r="S25" s="11"/>
+      <c r="T25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), T13, U13, 0 ) )</f>
         <v>2.411491593688377</v>
       </c>
-      <c r="U25" s="20"/>
-      <c r="V25" s="18">
+      <c r="U25" s="16"/>
+      <c r="V25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), V13, W13, 0 ) )</f>
         <v>1.2965615460910569</v>
       </c>
-      <c r="W25" s="18"/>
-      <c r="X25" s="20">
+      <c r="W25" s="11"/>
+      <c r="X25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), X13, Y13, 0 ) )</f>
         <v>0.91567814574715556</v>
       </c>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="18">
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), Z13, AA13, 0 ) )</f>
         <v>1.5429788757167571</v>
       </c>
-      <c r="AA25" s="18"/>
-      <c r="AB25" s="20">
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="16">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), AB13, AC13, 0 ) )</f>
         <v>0.73976437341199108</v>
       </c>
-      <c r="AC25" s="20"/>
-      <c r="AD25" s="18">
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="11">
         <f>LN( _xlfn.NORM.DIST( LN($AK13), AD13, AE13, 0 ) )</f>
         <v>1.4680077209757174</v>
       </c>
-      <c r="AE25" s="18"/>
+      <c r="AE25" s="11"/>
     </row>
     <row r="26" spans="1:36" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="18" t="e">
+      <c r="B26" s="11">
         <f t="shared" ref="B26:B32" si="0">LN( _xlfn.NORM.DIST( LN($AK14), B14, C14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="20" t="e">
+        <v>2.3835672893177455</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="16">
         <f t="shared" ref="D26:D32" si="1">LN( _xlfn.NORM.DIST( LN($AK14), D14, E14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F26" s="18" t="e">
+        <v>1.4228223016453769</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="11">
         <f t="shared" ref="F26:F32" si="2">LN( _xlfn.NORM.DIST( LN($AK14), F14, G14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="20" t="e">
+        <v>1.9615735008937081</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="16">
         <f t="shared" ref="H26:H32" si="3">LN( _xlfn.NORM.DIST( LN($AK14), H14, I14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="J26" s="18" t="e">
+        <v>1.799278344079914</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="11">
         <f t="shared" ref="J26:J32" si="4">LN( _xlfn.NORM.DIST( LN($AK14), J14, K14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="20" t="e">
+        <v>1.4856771575152299</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="16">
         <f t="shared" ref="L26:L32" si="5">LN( _xlfn.NORM.DIST( LN($AK14), L14, M14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N26" s="18" t="e">
+        <v>1.3096588778011666</v>
+      </c>
+      <c r="M26" s="3"/>
+      <c r="N26" s="11">
         <f t="shared" ref="N26:N32" si="6">LN( _xlfn.NORM.DIST( LN($AK14), N14, O14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O26" s="18"/>
-      <c r="P26" s="20" t="e">
+        <v>1.7209275637143335</v>
+      </c>
+      <c r="O26" s="11"/>
+      <c r="P26" s="16">
         <f t="shared" ref="P26:P32" si="7">LN( _xlfn.NORM.DIST( LN($AK14), P14, Q14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R26" s="18" t="e">
+        <v>1.4894315004693801</v>
+      </c>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="11">
         <f t="shared" ref="R26:R32" si="8">LN( _xlfn.NORM.DIST( LN($AK14), R14, S14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="S26" s="18"/>
-      <c r="T26" s="20" t="e">
+        <v>1.236395815726407</v>
+      </c>
+      <c r="S26" s="11"/>
+      <c r="T26" s="16">
         <f t="shared" ref="T26:T32" si="9">LN( _xlfn.NORM.DIST( LN($AK14), T14, U14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="V26" s="18" t="e">
+        <v>2.6791770455527617</v>
+      </c>
+      <c r="U26" s="3"/>
+      <c r="V26" s="11">
         <f t="shared" ref="V26:V32" si="10">LN( _xlfn.NORM.DIST( LN($AK14), V14, W14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W26" s="18"/>
-      <c r="X26" s="20" t="e">
+        <v>-5.08483150028558E-3</v>
+      </c>
+      <c r="W26" s="11"/>
+      <c r="X26" s="16">
         <f t="shared" ref="X26" si="11">LN( _xlfn.NORM.DIST( LN($AK14), X14, Y14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z26" s="18" t="e">
+        <v>1.3203869359022427</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="11">
         <f t="shared" ref="Z26:Z32" si="12">LN( _xlfn.NORM.DIST( LN($AK14), Z14, AA14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AA26" s="18"/>
-      <c r="AB26" s="20" t="e">
+        <v>1.3334141362179457</v>
+      </c>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="16">
         <f t="shared" ref="AB26" si="13">LN( _xlfn.NORM.DIST( LN($AK14), AB14, AC14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AD26" s="18" t="e">
+        <v>1.0070352780618763</v>
+      </c>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="11">
         <f t="shared" ref="AD26:AD32" si="14">LN( _xlfn.NORM.DIST( LN($AK14), AD14, AE14, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AE26" s="18"/>
+        <v>2.0811556796584072</v>
+      </c>
+      <c r="AE26" s="11"/>
     </row>
     <row r="27" spans="1:36" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">

</xml_diff>

<commit_message>
Scores Round 4 and updates for Round 5
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/Face2Face/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F6754D-87AF-D149-96A2-30A6AC6536A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E0B005-E85B-5944-BF87-D738211011D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30520" yWindow="-2400" windowWidth="30420" windowHeight="17080" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="30840" yWindow="-2400" windowWidth="33460" windowHeight="17820" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>mean</t>
   </si>
@@ -145,13 +145,16 @@
   </si>
   <si>
     <t>24th Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.265261	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,12 +240,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -306,9 +303,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967CD6C7-451E-0748-9748-9A42CF32D73A}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="96" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,10 +647,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>7</v>
@@ -708,63 +707,63 @@
       </c>
       <c r="B2" s="16">
         <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
-        <v>6.6735020985528868</v>
+        <v>8.6780629780107716</v>
       </c>
       <c r="C2" s="16">
+        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
+        <v>7.2263285012371785</v>
+      </c>
+      <c r="D2" s="16">
         <f>SUMIF($J25:$J34,"&lt;&gt;#NUM!")</f>
-        <v>5.0129024770659667</v>
-      </c>
-      <c r="D2" s="16">
-        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
-        <v>4.9671898363166793</v>
+        <v>6.5778357925684352</v>
       </c>
       <c r="E2" s="16">
         <f>SUMIF($L25:$L34,"&lt;&gt;#NUM!")</f>
-        <v>4.4002978232879828</v>
+        <v>6.44671212633836</v>
       </c>
       <c r="F2" s="16">
         <f>SUMIF($T25:$T34,"&lt;&gt;#NUM!")</f>
-        <v>4.3173944632168775</v>
+        <v>6.2704631513435629</v>
       </c>
       <c r="G2" s="16">
         <f>SUMIF($AD25:$AD34,"&lt;&gt;#NUM!")</f>
-        <v>4.1132140734950324</v>
+        <v>6.1332435951223747</v>
       </c>
       <c r="H2" s="16">
         <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>3.8980973883683929</v>
+        <v>5.7834816470446411</v>
       </c>
       <c r="I2" s="16">
         <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
-        <v>3.7067384821357283</v>
+        <v>5.5256775595157785</v>
       </c>
       <c r="J2" s="16">
         <f>SUMIF($Z25:$Z34,"&lt;&gt;#NUM!")</f>
-        <v>3.1918883938649754</v>
+        <v>5.1213455972835265</v>
       </c>
       <c r="K2" s="16">
         <f>SUMIF($AB25:$AB34,"&lt;&gt;#NUM!")</f>
-        <v>2.8608536915040941</v>
+        <v>4.6142716738709693</v>
       </c>
       <c r="L2" s="16">
         <f>SUMIF($D25:$D34,"&lt;&gt;#NUM!")</f>
-        <v>2.00869450442078</v>
+        <v>3.56093051258773</v>
       </c>
       <c r="M2" s="16">
         <f>SUMIF($R25:$R34,"&lt;&gt;#NUM!")</f>
-        <v>1.2937340265532216</v>
+        <v>3.364821923740029</v>
       </c>
       <c r="N2" s="16">
         <f>SUMIF($N25:$N34,"&lt;&gt;#NUM!")</f>
-        <v>0.22142706473492124</v>
+        <v>1.0054095703711634</v>
       </c>
       <c r="O2" s="16">
         <f>SUMIF($V25:$V34,"&lt;&gt;#NUM!")</f>
-        <v>-2.6910595707839282</v>
+        <v>-0.43461295338194228</v>
       </c>
       <c r="P2" s="16">
         <f>SUMIF($X25:$X34,"&lt;&gt;#NUM!")</f>
-        <v>-17.919673303803549</v>
+        <v>-15.630080110956731</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -1051,7 +1050,7 @@
       <c r="O13" s="10">
         <v>5.2329924722341999E-2</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="27">
         <v>10.28497</v>
       </c>
       <c r="Q13" s="4">
@@ -1063,7 +1062,7 @@
       <c r="S13" s="10">
         <v>4.6036359999999998E-2</v>
       </c>
-      <c r="T13" s="28">
+      <c r="T13" s="27">
         <v>10.259888249999999</v>
       </c>
       <c r="U13" s="4">
@@ -1075,7 +1074,7 @@
       <c r="W13" s="10">
         <v>9.6529813811318199E-2</v>
       </c>
-      <c r="X13" s="28">
+      <c r="X13" s="27">
         <v>10.291</v>
       </c>
       <c r="Y13" s="4">
@@ -1087,7 +1086,7 @@
       <c r="AA13" s="10">
         <v>6.6113560000000002E-2</v>
       </c>
-      <c r="AB13" s="28">
+      <c r="AB13" s="27">
         <v>10.143990000000001</v>
       </c>
       <c r="AC13" s="4">
@@ -1099,7 +1098,7 @@
       <c r="AE13" s="10">
         <v>7.4385259999999995E-2</v>
       </c>
-      <c r="AJ13" s="27" t="s">
+      <c r="AJ13" s="26" t="s">
         <v>29</v>
       </c>
       <c r="AK13" s="3">
@@ -1200,7 +1199,7 @@
       <c r="AE14" s="10">
         <v>4.5309839999999997E-2</v>
       </c>
-      <c r="AJ14" s="27" t="s">
+      <c r="AJ14" s="26" t="s">
         <v>30</v>
       </c>
       <c r="AK14" s="3">
@@ -1301,7 +1300,7 @@
       <c r="AE15" s="11">
         <v>4.5327600000000003E-2</v>
       </c>
-      <c r="AJ15" s="27" t="s">
+      <c r="AJ15" s="26" t="s">
         <v>31</v>
       </c>
       <c r="AK15" s="3">
@@ -1312,52 +1311,198 @@
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AJ16" s="27" t="s">
+      <c r="B16" s="11">
+        <v>10.20144</v>
+      </c>
+      <c r="C16" s="11">
+        <v>3.596862E-2</v>
+      </c>
+      <c r="D16" s="28">
+        <v>10.249309999999999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>10.214672858288401</v>
+      </c>
+      <c r="G16" s="11">
+        <v>3.63416893528569E-2</v>
+      </c>
+      <c r="H16" s="11">
+        <v>10.198689999999999</v>
+      </c>
+      <c r="I16" s="11">
+        <v>4.4369899999999997E-2</v>
+      </c>
+      <c r="J16" s="11">
+        <v>10.18465</v>
+      </c>
+      <c r="K16" s="11">
+        <v>5.9209999999999999E-2</v>
+      </c>
+      <c r="L16" s="11">
+        <v>10.21219</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4.6275509999999999E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <v>10.1510497944556</v>
+      </c>
+      <c r="O16" s="11">
+        <v>5.2304376908233703E-2</v>
+      </c>
+      <c r="P16" s="11">
+        <v>10.19636</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>4.7570000000000001E-2</v>
+      </c>
+      <c r="R16" s="11">
+        <v>10.22339</v>
+      </c>
+      <c r="S16" s="11">
+        <v>4.9199039999999999E-2</v>
+      </c>
+      <c r="T16" s="11">
+        <v>10.25763321</v>
+      </c>
+      <c r="U16" s="11">
+        <v>5.05812556616261E-2</v>
+      </c>
+      <c r="V16" s="11">
+        <v>10.23535</v>
+      </c>
+      <c r="W16" s="11">
+        <v>4.1744429999999999E-2</v>
+      </c>
+      <c r="X16" s="11">
+        <v>10.256467000000001</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>3.06587360736197E-2</v>
+      </c>
+      <c r="Z16" s="11">
+        <v>10.23462</v>
+      </c>
+      <c r="AA16" s="11">
+        <v>5.7929500000000002E-2</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>10.210129999999999</v>
+      </c>
+      <c r="AC16" s="11">
+        <v>6.4656519999999995E-2</v>
+      </c>
+      <c r="AD16" s="11">
+        <v>10.208399999999999</v>
+      </c>
+      <c r="AE16" s="11">
+        <v>4.5287899999999999E-2</v>
+      </c>
+      <c r="AJ16" s="26" t="s">
         <v>32</v>
+      </c>
+      <c r="AK16" s="3">
+        <v>27824.604169999999</v>
       </c>
     </row>
     <row r="17" spans="1:36" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AJ17" s="27" t="s">
+      <c r="B17" s="11">
+        <v>10.19042</v>
+      </c>
+      <c r="C17" s="11">
+        <v>3.6378519999999998E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>10.236700000000001</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F17" s="11">
+        <v>10.2419250636183</v>
+      </c>
+      <c r="G17" s="11">
+        <v>3.5642144545014999E-2</v>
+      </c>
+      <c r="H17" s="11">
+        <v>10.279199999999999</v>
+      </c>
+      <c r="I17" s="11">
+        <v>4.2956630000000003E-2</v>
+      </c>
+      <c r="J17" s="11">
+        <v>10.24614</v>
+      </c>
+      <c r="K17" s="11">
+        <v>5.926E-2</v>
+      </c>
+      <c r="L17" s="11">
+        <v>10.22756</v>
+      </c>
+      <c r="M17" s="11">
+        <v>4.3010199999999998E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <v>10.2776030649727</v>
+      </c>
+      <c r="O17" s="11">
+        <v>5.1385950965235697E-2</v>
+      </c>
+      <c r="P17" s="11">
+        <v>10.26464</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>4.7570000000000001E-2</v>
+      </c>
+      <c r="R17" s="11">
+        <v>10.286530000000001</v>
+      </c>
+      <c r="S17" s="11">
+        <v>4.9196810000000001E-2</v>
+      </c>
+      <c r="T17" s="11">
+        <v>10.24351747</v>
+      </c>
+      <c r="U17" s="11">
+        <v>2.4158716034764799E-2</v>
+      </c>
+      <c r="V17" s="11">
+        <v>10.237159999999999</v>
+      </c>
+      <c r="W17" s="11">
+        <v>4.1715519999999999E-2</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y17" s="11">
+        <v>3.0697423849999999E-2</v>
+      </c>
+      <c r="Z17" s="11">
+        <v>10.226533999999999</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>4.5451142999999999E-2</v>
+      </c>
+      <c r="AB17" s="11">
+        <v>10.147069999999999</v>
+      </c>
+      <c r="AC17" s="11">
+        <v>6.6359570000000007E-2</v>
+      </c>
+      <c r="AD17" s="11">
+        <v>10.267480000000001</v>
+      </c>
+      <c r="AE17" s="11">
+        <v>4.5286300000000002E-2</v>
+      </c>
+      <c r="AJ17" s="26" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1393,7 +1538,7 @@
       <c r="AC18" s="20"/>
       <c r="AD18" s="18"/>
       <c r="AE18" s="18"/>
-      <c r="AJ18" s="27" t="s">
+      <c r="AJ18" s="26" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1417,7 +1562,7 @@
       <c r="AA19" s="18"/>
       <c r="AD19" s="18"/>
       <c r="AE19" s="18"/>
-      <c r="AJ19" s="27" t="s">
+      <c r="AJ19" s="26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1445,7 +1590,7 @@
       <c r="AA20" s="18"/>
       <c r="AD20" s="18"/>
       <c r="AE20" s="18"/>
-      <c r="AJ20" s="27" t="s">
+      <c r="AJ20" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1813,72 +1958,72 @@
       <c r="A28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="18" t="e">
+      <c r="B28" s="18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>2.0045608794578844</v>
       </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="20" t="e">
+      <c r="D28" s="20">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F28" s="18" t="e">
+        <v>1.55223600816695</v>
+      </c>
+      <c r="F28" s="18">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>2.2591386649204996</v>
       </c>
       <c r="G28" s="18"/>
-      <c r="H28" s="20" t="e">
+      <c r="H28" s="20">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J28" s="18" t="e">
+        <v>1.8853842586762484</v>
+      </c>
+      <c r="J28" s="18">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
+        <v>1.5649333155024687</v>
       </c>
       <c r="K28" s="18"/>
-      <c r="L28" s="20" t="e">
+      <c r="L28" s="20">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N28" s="18" t="e">
+        <v>2.0464143030503767</v>
+      </c>
+      <c r="N28" s="18">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>0.78398250563624228</v>
       </c>
       <c r="O28" s="18"/>
-      <c r="P28" s="20" t="e">
+      <c r="P28" s="20">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R28" s="18" t="e">
+        <v>1.8189390773800505</v>
+      </c>
+      <c r="R28" s="18">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
+        <v>2.0710878971868074</v>
       </c>
       <c r="S28" s="18"/>
-      <c r="T28" s="20" t="e">
+      <c r="T28" s="20">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="V28" s="18" t="e">
+        <v>1.953068688126685</v>
+      </c>
+      <c r="V28" s="18">
         <f t="shared" si="10"/>
-        <v>#NUM!</v>
+        <v>2.2564466174019859</v>
       </c>
       <c r="W28" s="18"/>
-      <c r="X28" s="20" t="e">
+      <c r="X28" s="20">
         <f t="shared" ref="X28" si="17">LN( _xlfn.NORM.DIST( LN($AK16), X16, Y16, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z28" s="18" t="e">
+        <v>2.2895931928468172</v>
+      </c>
+      <c r="Z28" s="18">
         <f t="shared" si="12"/>
-        <v>#NUM!</v>
+        <v>1.9294572034185511</v>
       </c>
       <c r="AA28" s="18"/>
-      <c r="AB28" s="20" t="e">
+      <c r="AB28" s="20">
         <f t="shared" ref="AB28" si="18">LN( _xlfn.NORM.DIST( LN($AK16), AB16, AC16, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AD28" s="18" t="e">
+        <v>1.753417982366875</v>
+      </c>
+      <c r="AD28" s="18">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>2.0200295216273427</v>
       </c>
       <c r="AE28" s="18"/>
     </row>

</xml_diff>

<commit_message>
Scores 7th Round + Forecasts 8th Round
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/Face2Face/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94B4B6-E373-1946-BAFC-0331ED3909E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA7EE4-7D35-9646-9F39-22D6A69EE138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36280" yWindow="-2400" windowWidth="26820" windowHeight="17860" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="31380" yWindow="-2400" windowWidth="35820" windowHeight="17860" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,12 +230,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
       <family val="2"/>
@@ -273,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,13 +292,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967CD6C7-451E-0748-9748-9A42CF32D73A}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,13 +636,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>20</v>
@@ -704,63 +696,63 @@
       </c>
       <c r="B2" s="16">
         <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
-        <v>11.565306327506162</v>
+        <v>14.061749273285114</v>
       </c>
       <c r="C2" s="16">
+        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
+        <v>11.367821556284975</v>
+      </c>
+      <c r="D2" s="16">
+        <f>SUMIF($Z25:$Z34,"&lt;&gt;#NUM!")</f>
+        <v>10.869688916928354</v>
+      </c>
+      <c r="E2" s="16">
         <f>SUMIF($J25:$J34,"&lt;&gt;#NUM!")</f>
-        <v>9.1670910318215117</v>
-      </c>
-      <c r="D2" s="16">
-        <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
-        <v>9.156810754262608</v>
-      </c>
-      <c r="E2" s="16">
-        <f>SUMIF($Z25:$Z34,"&lt;&gt;#NUM!")</f>
-        <v>8.4561024199676513</v>
+        <v>10.798463966012594</v>
       </c>
       <c r="F2" s="16">
         <f>SUMIF($AD25:$AD34,"&lt;&gt;#NUM!")</f>
-        <v>7.8406576431600268</v>
+        <v>10.017830036429714</v>
       </c>
       <c r="G2" s="16">
         <f>SUMIF($L25:$L34,"&lt;&gt;#NUM!")</f>
-        <v>7.6587263393778322</v>
+        <v>9.8131177031910486</v>
       </c>
       <c r="H2" s="16">
         <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
-        <v>7.6487189859273625</v>
+        <v>9.5518034192997039</v>
       </c>
       <c r="I2" s="16">
         <f>SUMIF($AB25:$AB34,"&lt;&gt;#NUM!")</f>
-        <v>7.2330893563535898</v>
+        <v>8.80390279979264</v>
       </c>
       <c r="J2" s="16">
         <f>SUMIF($D25:$D34,"&lt;&gt;#NUM!")</f>
-        <v>6.0393835259908775</v>
+        <v>7.7388349823601423</v>
       </c>
       <c r="K2" s="16">
         <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>4.5761306672514159</v>
+        <v>6.43786499074701</v>
       </c>
       <c r="L2" s="16">
         <f>SUMIF($R25:$R34,"&lt;&gt;#NUM!")</f>
-        <v>1.6305516810697971</v>
+        <v>3.8403493058275466</v>
       </c>
       <c r="M2" s="16">
         <f>SUMIF($N25:$N34,"&lt;&gt;#NUM!")</f>
-        <v>1.4142064911251278</v>
+        <v>3.337421503497342</v>
       </c>
       <c r="N2" s="16">
         <f>SUMIF($T25:$T34,"&lt;&gt;#NUM!")</f>
-        <v>0.44997479769067539</v>
+        <v>2.4275012383147287</v>
       </c>
       <c r="O2" s="16">
         <f>SUMIF($V25:$V34,"&lt;&gt;#NUM!")</f>
-        <v>-0.83048413326470594</v>
+        <v>1.5744867627426766</v>
       </c>
       <c r="P2" s="16">
         <f>SUMIF($X25:$X34,"&lt;&gt;#NUM!")</f>
-        <v>-14.376727697730249</v>
+        <v>-18.061064520462686</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -1047,7 +1039,7 @@
       <c r="O13" s="10">
         <v>5.2329924722341999E-2</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="26">
         <v>10.28497</v>
       </c>
       <c r="Q13" s="15">
@@ -1059,7 +1051,7 @@
       <c r="S13" s="10">
         <v>4.6036359999999998E-2</v>
       </c>
-      <c r="T13" s="28">
+      <c r="T13" s="26">
         <v>10.259888249999999</v>
       </c>
       <c r="U13" s="15">
@@ -1071,7 +1063,7 @@
       <c r="W13" s="10">
         <v>9.6529813811318199E-2</v>
       </c>
-      <c r="X13" s="28">
+      <c r="X13" s="26">
         <v>10.291</v>
       </c>
       <c r="Y13" s="15">
@@ -1083,7 +1075,7 @@
       <c r="AA13" s="10">
         <v>6.6113560000000002E-2</v>
       </c>
-      <c r="AB13" s="28">
+      <c r="AB13" s="26">
         <v>10.143990000000001</v>
       </c>
       <c r="AC13" s="15">
@@ -1095,7 +1087,7 @@
       <c r="AE13" s="10">
         <v>7.4385259999999995E-2</v>
       </c>
-      <c r="AJ13" s="26" t="s">
+      <c r="AJ13" s="24" t="s">
         <v>29</v>
       </c>
       <c r="AK13" s="3">
@@ -1196,7 +1188,7 @@
       <c r="AE14" s="10">
         <v>4.5309839999999997E-2</v>
       </c>
-      <c r="AJ14" s="26" t="s">
+      <c r="AJ14" s="24" t="s">
         <v>30</v>
       </c>
       <c r="AK14" s="3">
@@ -1297,7 +1289,7 @@
       <c r="AE15" s="11">
         <v>4.5327600000000003E-2</v>
       </c>
-      <c r="AJ15" s="26" t="s">
+      <c r="AJ15" s="24" t="s">
         <v>31</v>
       </c>
       <c r="AK15" s="3">
@@ -1314,7 +1306,7 @@
       <c r="C16" s="11">
         <v>3.596862E-2</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="25">
         <v>10.249309999999999</v>
       </c>
       <c r="E16" s="3">
@@ -1398,7 +1390,7 @@
       <c r="AE16" s="11">
         <v>4.5287899999999999E-2</v>
       </c>
-      <c r="AJ16" s="26" t="s">
+      <c r="AJ16" s="24" t="s">
         <v>32</v>
       </c>
       <c r="AK16" s="3">
@@ -1499,7 +1491,7 @@
       <c r="AE17" s="11">
         <v>4.5286300000000002E-2</v>
       </c>
-      <c r="AJ17" s="26" t="s">
+      <c r="AJ17" s="24" t="s">
         <v>33</v>
       </c>
       <c r="AK17" s="3">
@@ -1519,7 +1511,7 @@
       <c r="D18" s="3">
         <v>10.07117</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="25">
         <v>0.06</v>
       </c>
       <c r="F18" s="11">
@@ -1600,7 +1592,7 @@
       <c r="AE18" s="11">
         <v>4.0331409999999998E-2</v>
       </c>
-      <c r="AJ18" s="26" t="s">
+      <c r="AJ18" s="24" t="s">
         <v>34</v>
       </c>
       <c r="AK18" s="3">
@@ -1611,51 +1603,198 @@
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AD19" s="18"/>
-      <c r="AE19" s="18"/>
-      <c r="AJ19" s="26" t="s">
+      <c r="B19" s="11">
+        <v>10.15448</v>
+      </c>
+      <c r="C19" s="11">
+        <v>3.2787620000000003E-2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>10.113</v>
+      </c>
+      <c r="E19" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>10.1715228989575</v>
+      </c>
+      <c r="G19" s="11">
+        <v>3.8591922612253499E-2</v>
+      </c>
+      <c r="H19" s="16">
+        <v>10.11476</v>
+      </c>
+      <c r="I19" s="16">
+        <v>3.9686220000000001E-2</v>
+      </c>
+      <c r="J19" s="11">
+        <v>10.108219999999999</v>
+      </c>
+      <c r="K19" s="11">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="L19" s="16">
+        <v>10.17572</v>
+      </c>
+      <c r="M19" s="16">
+        <v>3.8370000000000001E-2</v>
+      </c>
+      <c r="N19" s="11">
+        <v>10.177890239162201</v>
+      </c>
+      <c r="O19" s="11">
+        <v>5.1502554437963401E-2</v>
+      </c>
+      <c r="P19" s="16">
+        <v>10.177110000000001</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>5.336693E-2</v>
+      </c>
+      <c r="R19" s="11">
+        <v>10.160299999999999</v>
+      </c>
+      <c r="S19" s="11">
+        <v>4.301224E-2</v>
+      </c>
+      <c r="T19" s="16">
+        <v>10.1833086</v>
+      </c>
+      <c r="U19" s="16">
+        <v>2.4158716034764799E-2</v>
+      </c>
+      <c r="V19" s="11">
+        <v>10.1637198081406</v>
+      </c>
+      <c r="W19" s="11">
+        <v>3.4020590900224003E-2</v>
+      </c>
+      <c r="X19" s="16">
+        <v>10.217287929625</v>
+      </c>
+      <c r="Y19" s="16">
+        <v>1.76327746252582E-2</v>
+      </c>
+      <c r="Z19" s="11">
+        <v>10.171804</v>
+      </c>
+      <c r="AA19" s="11">
+        <v>2.7948322698303201E-2</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>10.192887600000001</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>7.0101046581429197E-2</v>
+      </c>
+      <c r="AD19" s="11">
+        <v>10.143330000000001</v>
+      </c>
+      <c r="AE19" s="11">
+        <v>4.4318910000000003E-2</v>
+      </c>
+      <c r="AJ19" s="24" t="s">
         <v>35</v>
+      </c>
+      <c r="AK19">
+        <v>25648.625</v>
       </c>
     </row>
     <row r="20" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AD20" s="18"/>
-      <c r="AE20" s="18"/>
-      <c r="AJ20" s="26" t="s">
+      <c r="B20" s="11">
+        <v>10.134169999999999</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3.3082220000000002E-2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10.140764000000001</v>
+      </c>
+      <c r="E20" s="3">
+        <v>6.0013259999999999E-2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>10.1490167666731</v>
+      </c>
+      <c r="G20" s="11">
+        <v>3.8214052298871301E-2</v>
+      </c>
+      <c r="H20" s="16">
+        <v>10.11416</v>
+      </c>
+      <c r="I20" s="16">
+        <v>4.03699E-2</v>
+      </c>
+      <c r="J20" s="11">
+        <v>10.14658</v>
+      </c>
+      <c r="K20" s="11">
+        <v>5.9290000000000002E-2</v>
+      </c>
+      <c r="L20" s="16">
+        <v>10.147629999999999</v>
+      </c>
+      <c r="M20" s="16">
+        <v>3.8321429999999997E-2</v>
+      </c>
+      <c r="N20" s="11">
+        <v>10.130065098065501</v>
+      </c>
+      <c r="O20" s="11">
+        <v>5.1608321964626898E-2</v>
+      </c>
+      <c r="P20" s="16">
+        <v>10.13753</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>5.3336630000000003E-2</v>
+      </c>
+      <c r="R20" s="11">
+        <v>10.152609999999999</v>
+      </c>
+      <c r="S20" s="11">
+        <v>4.298888E-2</v>
+      </c>
+      <c r="T20" s="16">
+        <v>10.14227064</v>
+      </c>
+      <c r="U20" s="16">
+        <v>3.8669870780580103E-2</v>
+      </c>
+      <c r="V20" s="11">
+        <v>10.1567557077405</v>
+      </c>
+      <c r="W20" s="11">
+        <v>3.40177985260579E-2</v>
+      </c>
+      <c r="X20" s="16">
+        <v>1.76327746252582E-2</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>1.9786818293756399E-2</v>
+      </c>
+      <c r="Z20" s="11">
+        <v>10.13943272</v>
+      </c>
+      <c r="AA20" s="11">
+        <v>3.7003501600000002E-2</v>
+      </c>
+      <c r="AB20" s="16">
+        <v>10.1528770494544</v>
+      </c>
+      <c r="AC20" s="16">
+        <v>8.1210083679188805E-2</v>
+      </c>
+      <c r="AD20" s="11">
+        <v>10.142300000000001</v>
+      </c>
+      <c r="AE20" s="11">
+        <v>4.5338690000000001E-2</v>
+      </c>
+      <c r="AJ20" s="24" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1909,7 +2048,7 @@
       </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="11">
-        <f t="shared" ref="R26:R32" si="8">LN( _xlfn.NORM.DIST( LN($AK14), R14, S14, 0 ) )</f>
+        <f t="shared" ref="R26:R31" si="8">LN( _xlfn.NORM.DIST( LN($AK14), R14, S14, 0 ) )</f>
         <v>1.236395815726407</v>
       </c>
       <c r="S26" s="11"/>
@@ -2268,72 +2407,79 @@
       <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="18" t="e">
+      <c r="B31" s="11">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="20" t="e">
+        <v>2.4964429457789521</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="16">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F31" s="18" t="e">
+        <v>1.6994514563692653</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="11">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="20" t="e">
+        <v>2.2110108020223667</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="16">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J31" s="18" t="e">
+        <v>1.8617343234955943</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="11">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="20" t="e">
+        <v>1.6313729341910816</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="16">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N31" s="18" t="e">
+        <v>2.1543913638132168</v>
+      </c>
+      <c r="M31" s="3"/>
+      <c r="N31" s="11">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O31" s="18"/>
-      <c r="P31" s="20" t="e">
+        <v>1.9232150123722143</v>
+      </c>
+      <c r="O31" s="11"/>
+      <c r="P31" s="16">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R31" s="18" t="e">
+        <v>1.9030844333723416</v>
+      </c>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="11">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S31" s="18"/>
-      <c r="T31" s="20" t="e">
+        <v>2.2097976247577495</v>
+      </c>
+      <c r="S31" s="11"/>
+      <c r="T31" s="16">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="V31" s="18" t="e">
+        <v>1.9775264406240534</v>
+      </c>
+      <c r="U31" s="3"/>
+      <c r="V31" s="11">
         <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="W31" s="18"/>
-      <c r="X31" s="20" t="e">
+        <v>2.4049708960073826</v>
+      </c>
+      <c r="W31" s="11"/>
+      <c r="X31" s="16">
         <f t="shared" ref="X31" si="22">LN( _xlfn.NORM.DIST( LN($AK19), X19, Y19, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z31" s="18" t="e">
+        <v>-3.6843368227324382</v>
+      </c>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="11">
         <f t="shared" si="12"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AA31" s="18"/>
-      <c r="AB31" s="20" t="e">
+        <v>2.4135864969607015</v>
+      </c>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="16">
         <f t="shared" ref="AB31" si="23">LN( _xlfn.NORM.DIST( LN($AK19), AB19, AC19, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AD31" s="18" t="e">
+        <v>1.5708134434390499</v>
+      </c>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="11">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>2.177172393269688</v>
       </c>
       <c r="AE31" s="18"/>
     </row>
@@ -2378,7 +2524,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R32" s="18" t="e">
-        <f t="shared" si="8"/>
+        <f>LN( _xlfn.NORM.DIST( LN($AK20), R20, S20, 0 ) )</f>
         <v>#NUM!</v>
       </c>
       <c r="S32" s="18"/>

</xml_diff>

<commit_message>
Final Scores, including scores without the worst forecast
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/Face2Face/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA7EE4-7D35-9646-9F39-22D6A69EE138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C839FDB0-DF7D-F34E-BDC2-27645955C7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="-2400" windowWidth="35820" windowHeight="17860" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="29840" yWindow="-380" windowWidth="35820" windowHeight="17860" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scores" sheetId="1" r:id="rId1"/>
+    <sheet name="Scores without the worst case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="39">
   <si>
     <t>mean</t>
   </si>
@@ -145,13 +146,19 @@
   </si>
   <si>
     <t>24th Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SORTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,8 +241,41 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -267,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,6 +343,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967CD6C7-451E-0748-9748-9A42CF32D73A}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,63 +756,63 @@
       </c>
       <c r="B2" s="16">
         <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
-        <v>14.061749273285114</v>
+        <v>16.46662997430904</v>
       </c>
       <c r="C2" s="16">
         <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
-        <v>11.367821556284975</v>
+        <v>13.712932512915343</v>
       </c>
       <c r="D2" s="16">
         <f>SUMIF($Z25:$Z34,"&lt;&gt;#NUM!")</f>
-        <v>10.869688916928354</v>
+        <v>13.221895058336258</v>
       </c>
       <c r="E2" s="16">
         <f>SUMIF($J25:$J34,"&lt;&gt;#NUM!")</f>
-        <v>10.798463966012594</v>
+        <v>12.704626494187691</v>
       </c>
       <c r="F2" s="16">
         <f>SUMIF($AD25:$AD34,"&lt;&gt;#NUM!")</f>
-        <v>10.017830036429714</v>
+        <v>12.185113777624386</v>
       </c>
       <c r="G2" s="16">
         <f>SUMIF($L25:$L34,"&lt;&gt;#NUM!")</f>
-        <v>9.8131177031910486</v>
+        <v>12.155914711708409</v>
       </c>
       <c r="H2" s="16">
         <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
-        <v>9.5518034192997039</v>
+        <v>11.54543968190103</v>
       </c>
       <c r="I2" s="16">
         <f>SUMIF($AB25:$AB34,"&lt;&gt;#NUM!")</f>
-        <v>8.80390279979264</v>
+        <v>10.393730013463333</v>
       </c>
       <c r="J2" s="16">
         <f>SUMIF($D25:$D34,"&lt;&gt;#NUM!")</f>
-        <v>7.7388349823601423</v>
+        <v>9.6262030585594864</v>
       </c>
       <c r="K2" s="16">
         <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>6.43786499074701</v>
+        <v>8.3812975243797716</v>
       </c>
       <c r="L2" s="16">
         <f>SUMIF($R25:$R34,"&lt;&gt;#NUM!")</f>
-        <v>3.8403493058275466</v>
+        <v>6.0619788436581343</v>
       </c>
       <c r="M2" s="16">
         <f>SUMIF($N25:$N34,"&lt;&gt;#NUM!")</f>
-        <v>3.337421503497342</v>
+        <v>5.3234740771733486</v>
       </c>
       <c r="N2" s="16">
         <f>SUMIF($T25:$T34,"&lt;&gt;#NUM!")</f>
-        <v>2.4275012383147287</v>
+        <v>4.7510145640117827</v>
       </c>
       <c r="O2" s="16">
         <f>SUMIF($V25:$V34,"&lt;&gt;#NUM!")</f>
-        <v>1.5744867627426766</v>
+        <v>4.0018066188339469</v>
       </c>
       <c r="P2" s="16">
         <f>SUMIF($X25:$X34,"&lt;&gt;#NUM!")</f>
-        <v>-18.061064520462686</v>
+        <v>-17.890606000516513</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -1771,7 +1831,7 @@
         <v>3.40177985260579E-2</v>
       </c>
       <c r="X20" s="16">
-        <v>1.76327746252582E-2</v>
+        <v>10.194907462110701</v>
       </c>
       <c r="Y20" s="15">
         <v>1.9786818293756399E-2</v>
@@ -1796,6 +1856,9 @@
       </c>
       <c r="AJ20" s="24" t="s">
         <v>36</v>
+      </c>
+      <c r="AK20">
+        <v>25535</v>
       </c>
     </row>
     <row r="21" spans="1:37" ht="20" x14ac:dyDescent="0.25">
@@ -1822,6 +1885,8 @@
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
       <c r="W21" s="20"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="16"/>
       <c r="Z21" s="20"/>
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
@@ -2463,7 +2528,7 @@
       </c>
       <c r="W31" s="11"/>
       <c r="X31" s="16">
-        <f t="shared" ref="X31" si="22">LN( _xlfn.NORM.DIST( LN($AK19), X19, Y19, 0 ) )</f>
+        <f t="shared" ref="X31:X32" si="22">LN( _xlfn.NORM.DIST( LN($AK19), X19, Y19, 0 ) )</f>
         <v>-3.6843368227324382</v>
       </c>
       <c r="Y31" s="3"/>
@@ -2487,72 +2552,72 @@
       <c r="A32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="18" t="e">
+      <c r="B32" s="18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>2.4048807010239268</v>
       </c>
       <c r="C32" s="18"/>
-      <c r="D32" s="20" t="e">
+      <c r="D32" s="20">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F32" s="18" t="e">
+        <v>1.8873680761993441</v>
+      </c>
+      <c r="F32" s="18">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>2.3451109566303674</v>
       </c>
       <c r="G32" s="18"/>
-      <c r="H32" s="20" t="e">
+      <c r="H32" s="20">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J32" s="18" t="e">
+        <v>1.9434325336327625</v>
+      </c>
+      <c r="J32" s="18">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
+        <v>1.9061625281750971</v>
       </c>
       <c r="K32" s="18"/>
-      <c r="L32" s="20" t="e">
+      <c r="L32" s="20">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N32" s="18" t="e">
+        <v>2.3427970085173602</v>
+      </c>
+      <c r="N32" s="18">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>1.9860525736760068</v>
       </c>
       <c r="O32" s="18"/>
-      <c r="P32" s="20" t="e">
+      <c r="P32" s="20">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R32" s="18" t="e">
+        <v>1.9936362626013253</v>
+      </c>
+      <c r="R32" s="18">
         <f>LN( _xlfn.NORM.DIST( LN($AK20), R20, S20, 0 ) )</f>
-        <v>#NUM!</v>
+        <v>2.2216295378305877</v>
       </c>
       <c r="S32" s="18"/>
-      <c r="T32" s="20" t="e">
+      <c r="T32" s="20">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="V32" s="18" t="e">
+        <v>2.3235133256970535</v>
+      </c>
+      <c r="V32" s="18">
         <f t="shared" si="10"/>
-        <v>#NUM!</v>
+        <v>2.4273198560912705</v>
       </c>
       <c r="W32" s="18"/>
-      <c r="X32" s="20" t="e">
-        <f>LN( _xlfn.NORM.DIST( LN($AK20), X21, Y21, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Z32" s="18" t="e">
+      <c r="X32" s="16">
+        <f t="shared" si="22"/>
+        <v>0.17045851994617234</v>
+      </c>
+      <c r="Z32" s="18">
         <f t="shared" si="12"/>
-        <v>#NUM!</v>
+        <v>2.3522061414079038</v>
       </c>
       <c r="AA32" s="18"/>
-      <c r="AB32" s="20" t="e">
+      <c r="AB32" s="20">
         <f t="shared" ref="AB32" si="24">LN( _xlfn.NORM.DIST( LN($AK20), AB20, AC20, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AD32" s="18" t="e">
+        <v>1.5898272136706928</v>
+      </c>
+      <c r="AD32" s="18">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>2.1672837411946717</v>
       </c>
       <c r="AE32" s="18"/>
     </row>
@@ -2629,4 +2694,1062 @@
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3122A1E-BF8D-D249-91D6-558A82C1A847}">
+  <dimension ref="A1:AE18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:31" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="30"/>
+      <c r="B1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="33"/>
+      <c r="L1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="32"/>
+      <c r="N1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="33"/>
+      <c r="P1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="33"/>
+      <c r="T1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="32"/>
+      <c r="V1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="33"/>
+      <c r="X1" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="27"/>
+    </row>
+    <row r="2" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="34">
+        <v>2.4964430000000002</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="35">
+        <v>1.8873680799999999</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="34">
+        <v>2.34511096</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="35">
+        <v>1.9434325299999999</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="34">
+        <v>1.90616253</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="35">
+        <v>2.3427970089999999</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="34">
+        <v>1.9860525739999999</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="35">
+        <v>1.993636263</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="34">
+        <v>2.2216295399999999</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="35">
+        <v>2.679177046</v>
+      </c>
+      <c r="U2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="34">
+        <v>2.427319856</v>
+      </c>
+      <c r="W2" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="35">
+        <v>2.289593</v>
+      </c>
+      <c r="Y2" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="34">
+        <v>2.413586</v>
+      </c>
+      <c r="AA2" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="35">
+        <v>1.7534179999999999</v>
+      </c>
+      <c r="AC2" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="34">
+        <v>2.1771720000000001</v>
+      </c>
+      <c r="AE2" s="29"/>
+    </row>
+    <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="34">
+        <v>2.4048807000000001</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="35">
+        <v>1.7846379999999999</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="34">
+        <v>2.2591389999999998</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1.899813</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="34">
+        <v>1.8219179999999999</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="35">
+        <v>2.1543913639999999</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="34">
+        <v>1.985557719</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="35">
+        <v>1.9030844330000001</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="34">
+        <v>2.2097980000000002</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="35">
+        <v>2.4114915940000001</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="34">
+        <v>2.404970896</v>
+      </c>
+      <c r="W3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="35">
+        <v>1.320387</v>
+      </c>
+      <c r="Y3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="34">
+        <v>2.3522061399999998</v>
+      </c>
+      <c r="AA3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="35">
+        <v>1.5898272099999999</v>
+      </c>
+      <c r="AC3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="34">
+        <v>2.1672837399999998</v>
+      </c>
+      <c r="AE3" s="29"/>
+    </row>
+    <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="34">
+        <v>2.3835670000000002</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="35">
+        <v>1.699451</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="34">
+        <v>2.2110110000000001</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="35">
+        <v>1.8853839999999999</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="34">
+        <v>1.7053069999999999</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="35">
+        <v>2.0970645399999999</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="34">
+        <v>1.923215012</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="35">
+        <v>1.818939077</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="34">
+        <v>2.071088</v>
+      </c>
+      <c r="S4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="35">
+        <v>2.323513326</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="34">
+        <v>2.2564466169999999</v>
+      </c>
+      <c r="W4" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="X4" s="35">
+        <v>0.91567799999999999</v>
+      </c>
+      <c r="Y4" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="34">
+        <v>2.0661360000000002</v>
+      </c>
+      <c r="AA4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB4" s="35">
+        <v>1.570813</v>
+      </c>
+      <c r="AC4" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="34">
+        <v>2.081156</v>
+      </c>
+      <c r="AE4" s="29"/>
+    </row>
+    <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="34">
+        <v>2.3207399999999998</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="35">
+        <v>1.5522359999999999</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="34">
+        <v>1.967044</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="35">
+        <v>1.861734</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="34">
+        <v>1.672912</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="35">
+        <v>2.0464143030000002</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="34">
+        <v>1.7209275639999999</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="35">
+        <v>1.4894315</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="34">
+        <v>1.2363960000000001</v>
+      </c>
+      <c r="S5" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="35">
+        <v>1.977526441</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="34">
+        <v>1.971802085</v>
+      </c>
+      <c r="W5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="35">
+        <v>0.67616299999999996</v>
+      </c>
+      <c r="Y5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="34">
+        <v>1.929457</v>
+      </c>
+      <c r="AA5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="35">
+        <v>1.4047229999999999</v>
+      </c>
+      <c r="AC5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD5" s="34">
+        <v>2.0200300000000002</v>
+      </c>
+      <c r="AE5" s="29"/>
+    </row>
+    <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="34">
+        <v>2.3077489999999998</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="35">
+        <v>1.422822</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="34">
+        <v>1.9615739999999999</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="35">
+        <v>1.7992779999999999</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="34">
+        <v>1.631373</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="35">
+        <v>1.75131098</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="34">
+        <v>1.0678093420000001</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="35">
+        <v>1.3711438979999999</v>
+      </c>
+      <c r="Q6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="34">
+        <v>0.948739</v>
+      </c>
+      <c r="S6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="35">
+        <v>1.9530686880000001</v>
+      </c>
+      <c r="U6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="34">
+        <v>1.296561546</v>
+      </c>
+      <c r="W6" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" s="35">
+        <v>0.57718899999999995</v>
+      </c>
+      <c r="Y6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z6" s="34">
+        <v>1.5429790000000001</v>
+      </c>
+      <c r="AA6" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" s="35">
+        <v>1.2140949999999999</v>
+      </c>
+      <c r="AC6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD6" s="34">
+        <v>1.468008</v>
+      </c>
+      <c r="AE6" s="29"/>
+    </row>
+    <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="34">
+        <v>2.0045609999999998</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="35">
+        <v>1.3817060000000001</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="34">
+        <v>1.896015</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="35">
+        <v>0.76093</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="34">
+        <v>1.5649329999999999</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="35">
+        <v>1.3393279650000001</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="34">
+        <v>0.78398250599999997</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="35">
+        <v>1.3564914589999999</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="R7" s="34">
+        <v>0.74001600000000001</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" s="35">
+        <v>1.5726430410000001</v>
+      </c>
+      <c r="U7" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="34">
+        <v>-5.0848320000000001E-3</v>
+      </c>
+      <c r="W7" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="X7" s="35">
+        <v>0.170459</v>
+      </c>
+      <c r="Y7" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z7" s="34">
+        <v>1.3334140000000001</v>
+      </c>
+      <c r="AA7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="35">
+        <v>1.1140540000000001</v>
+      </c>
+      <c r="AC7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD7" s="34">
+        <v>1.2423379999999999</v>
+      </c>
+      <c r="AE7" s="29"/>
+    </row>
+    <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1.969195</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="35">
+        <v>0.69381499999999996</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="34">
+        <v>1.038573</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0.19900599999999999</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="34">
+        <v>1.4856769999999999</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="35">
+        <v>1.309658878</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="34">
+        <v>-0.65901242199999999</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="35">
+        <v>0.84616308399999995</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="34">
+        <v>-0.891401</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="35">
+        <v>-0.77327418000000003</v>
+      </c>
+      <c r="U8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="34">
+        <v>-2.3676732650000001</v>
+      </c>
+      <c r="W8" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="X8" s="35">
+        <v>-3.6843370000000002</v>
+      </c>
+      <c r="Y8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" s="34">
+        <v>1.268621</v>
+      </c>
+      <c r="AA8" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB8" s="35">
+        <v>1.0070349999999999</v>
+      </c>
+      <c r="AC8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD8" s="34">
+        <v>0.56405099999999997</v>
+      </c>
+      <c r="AE8" s="28"/>
+    </row>
+    <row r="9" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="34">
+        <v>0.57949399999999995</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="35">
+        <v>-0.79583400000000004</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="34">
+        <v>3.4467999999999999E-2</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="35">
+        <v>-1.9682809999999999</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.91634400000000005</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="35">
+        <v>-0.88505032699999997</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="34">
+        <v>-3.4850582179999998</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="35">
+        <v>0.766549967</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="34">
+        <v>-2.4742869999999999</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="35">
+        <v>-7.3931313899999997</v>
+      </c>
+      <c r="U9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="34">
+        <v>-3.9825362850000001</v>
+      </c>
+      <c r="W9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" s="35">
+        <v>-20.155740000000002</v>
+      </c>
+      <c r="Y9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z9" s="34">
+        <v>0.31549500000000003</v>
+      </c>
+      <c r="AA9" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB9" s="35">
+        <v>0.73976399999999998</v>
+      </c>
+      <c r="AC9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD9" s="34">
+        <v>0.46507599999999999</v>
+      </c>
+      <c r="AE9" s="28"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AD11" s="36"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B12" s="36">
+        <f>SUM(B2:B8)</f>
+        <v>15.887135699999998</v>
+      </c>
+      <c r="C12" s="36">
+        <f>SUM(D2:D8)</f>
+        <v>10.42203608</v>
+      </c>
+      <c r="D12" s="36">
+        <f>SUM(F2:F8)</f>
+        <v>13.67846696</v>
+      </c>
+      <c r="E12" s="36">
+        <f>SUM(H2:H8)</f>
+        <v>10.349577530000001</v>
+      </c>
+      <c r="F12" s="36">
+        <f>SUM(J2:J8)</f>
+        <v>11.78828253</v>
+      </c>
+      <c r="G12" s="36">
+        <f>SUM(L2:L8)</f>
+        <v>13.040965039000001</v>
+      </c>
+      <c r="H12" s="36">
+        <f>SUM(N2:N8)</f>
+        <v>8.8085322949999991</v>
+      </c>
+      <c r="I12" s="36">
+        <f>SUM(P2:P8)</f>
+        <v>10.778889714000002</v>
+      </c>
+      <c r="J12" s="36">
+        <f>SUM(R2:R8)</f>
+        <v>8.5362655400000005</v>
+      </c>
+      <c r="K12" s="36">
+        <f>SUM(T2:T8)</f>
+        <v>12.144145956000001</v>
+      </c>
+      <c r="L12" s="36">
+        <f>SUM(V2:V8)</f>
+        <v>7.9843429029999999</v>
+      </c>
+      <c r="M12" s="36">
+        <f>SUM(X2:X8)</f>
+        <v>2.2651319999999995</v>
+      </c>
+      <c r="N12" s="36">
+        <f>SUM(Z2:Z8)</f>
+        <v>12.90639914</v>
+      </c>
+      <c r="O12" s="36">
+        <f>SUM(AB2:AB8)</f>
+        <v>9.6539652099999991</v>
+      </c>
+      <c r="P12" s="36">
+        <f>SUM(AD2:AD8)</f>
+        <v>11.720038739999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14" s="37"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="40">
+        <v>15.887135699999998</v>
+      </c>
+      <c r="C15" s="40">
+        <v>13.67846696</v>
+      </c>
+      <c r="D15" s="40">
+        <v>13.040965039000001</v>
+      </c>
+      <c r="E15" s="40">
+        <v>12.90639914</v>
+      </c>
+      <c r="F15" s="40">
+        <v>12.144145956000001</v>
+      </c>
+      <c r="G15" s="40">
+        <v>11.78828253</v>
+      </c>
+      <c r="H15" s="40">
+        <v>11.720038739999998</v>
+      </c>
+      <c r="I15" s="40">
+        <v>10.778889714000002</v>
+      </c>
+      <c r="J15" s="40">
+        <v>10.42203608</v>
+      </c>
+      <c r="K15" s="40">
+        <v>10.349577530000001</v>
+      </c>
+      <c r="L15" s="40">
+        <v>9.6539652099999991</v>
+      </c>
+      <c r="M15" s="40">
+        <v>8.8085322949999991</v>
+      </c>
+      <c r="N15" s="40">
+        <v>8.5362655400000005</v>
+      </c>
+      <c r="O15" s="40">
+        <v>7.9843429029999999</v>
+      </c>
+      <c r="P15" s="40">
+        <v>2.2651319999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="30:30" x14ac:dyDescent="0.2">
+      <c r="AD18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B14:P15">
+    <sortCondition descending="1" ref="B15:P15"/>
+  </sortState>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>